<commit_message>
Changed 'list_of_dishes' array to 'menu'
</commit_message>
<xml_diff>
--- a/takeaway_dm.xlsx
+++ b/takeaway_dm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HD - Data/Users/student/projects/makers_onsite/week_2/takeaway-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AB1670-7F77-6D44-832C-E172173AEC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6E1DD6-D20B-9B47-9774-983B88726A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="2" xr2:uid="{EE46B6FD-0BC1-D04E-BA86-FA1CEC1272BB}"/>
+    <workbookView xWindow="-980" yWindow="-23540" windowWidth="33660" windowHeight="18400" activeTab="2" xr2:uid="{EE46B6FD-0BC1-D04E-BA86-FA1CEC1272BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Creating a repository" sheetId="2" r:id="rId1"/>
@@ -145,9 +145,6 @@
     <t>Menu</t>
   </si>
   <si>
-    <t>@dishes --&gt; this is storing the list of dishes</t>
-  </si>
-  <si>
     <t>add_dish(new_dish)</t>
   </si>
   <si>
@@ -158,17 +155,20 @@
   </si>
   <si>
     <t>Saving price to dish_price in Dishes class</t>
+  </si>
+  <si>
+    <t>Adding hash with dish_name and dish_price in list_of_dishes array</t>
   </si>
   <si>
     <t>add_dish(new_dish)
 add_price(price)
-combine_list</t>
-  </si>
-  <si>
-    <t>combine_list</t>
-  </si>
-  <si>
-    <t>Adding hash with dish_name and dish_price in list_of_dishes array</t>
+add_to_menu</t>
+  </si>
+  <si>
+    <t>@menu --&gt; this is storing the list of dishes</t>
+  </si>
+  <si>
+    <t>add_to_menu</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF9A947-352B-C74E-9AC0-44D811991EBC}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="61" thickBot="1" x14ac:dyDescent="0.3">
@@ -1237,10 +1237,10 @@
         <v>32</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="61" thickBot="1" x14ac:dyDescent="0.3">
@@ -1258,10 +1258,10 @@
         <v>32</v>
       </c>
       <c r="H19" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I19" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="80" x14ac:dyDescent="0.25">
@@ -1273,10 +1273,10 @@
         <v>32</v>
       </c>
       <c r="H20" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I20" s="47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added empty User class
</commit_message>
<xml_diff>
--- a/takeaway_dm.xlsx
+++ b/takeaway_dm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HD - Data/Users/student/projects/makers_onsite/week_2/takeaway-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6E1DD6-D20B-9B47-9774-983B88726A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1EF575-2996-9F4D-835A-B5148AFBD24F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-980" yWindow="-23540" windowWidth="33660" windowHeight="18400" activeTab="2" xr2:uid="{EE46B6FD-0BC1-D04E-BA86-FA1CEC1272BB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="2" xr2:uid="{EE46B6FD-0BC1-D04E-BA86-FA1CEC1272BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Creating a repository" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
   <si>
     <t>Attributes</t>
   </si>
@@ -169,13 +169,25 @@
   </si>
   <si>
     <t>add_to_menu</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Basket</t>
+  </si>
+  <si>
+    <t>@display_menu from Menu class</t>
+  </si>
+  <si>
+    <t>displays menu for user to choose from</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,6 +221,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -475,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -531,16 +551,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -557,10 +572,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -598,6 +609,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,21 +1091,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF9A947-352B-C74E-9AC0-44D811991EBC}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="16"/>
-    <col min="3" max="3" width="13.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61" style="15" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="15" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="15" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="15"/>
-    <col min="7" max="7" width="19.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.83203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.83203125" style="15" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1088,7 +1127,7 @@
       <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="34" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="19"/>
@@ -1101,7 +1140,7 @@
       <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="25" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="19"/>
@@ -1114,7 +1153,7 @@
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="19"/>
@@ -1127,7 +1166,7 @@
       <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="25" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="19"/>
@@ -1149,13 +1188,13 @@
     </row>
     <row r="10" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="50" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="50" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="20" t="s">
@@ -1163,206 +1202,302 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="G12" s="26" t="s">
+      <c r="D12" s="24"/>
+      <c r="G12" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="35" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="61" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="12">
+    <row r="14" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="53"/>
+      <c r="D14" s="44"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="43"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="45"/>
+      <c r="G16" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="2:9" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="36"/>
+    </row>
+    <row r="18" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12">
         <v>3</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="12" t="s">
+    <row r="20" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:9" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D21" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E21" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="12" t="s">
+      <c r="F21" s="17"/>
+      <c r="G21" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H21" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I21" s="49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="C18" s="29" t="s">
+    <row r="22" spans="2:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="C22" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D22" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E22" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="29" t="s">
+      <c r="F22" s="17"/>
+      <c r="G22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="H22" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="31" t="s">
+      <c r="I22" s="28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="61" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="32" t="s">
+    <row r="23" spans="2:9" ht="61" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D23" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E23" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="45" t="s">
+      <c r="F23" s="22"/>
+      <c r="G23" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="46" t="s">
+      <c r="H23" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="47" t="s">
+      <c r="I23" s="42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="80" x14ac:dyDescent="0.25">
-      <c r="C20" s="42"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="45" t="s">
+    <row r="24" spans="2:9" ht="80" x14ac:dyDescent="0.25">
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="46" t="s">
+      <c r="H24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I24" s="42" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="12">
+    <row r="25" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="46"/>
+    </row>
+    <row r="26" spans="2:9" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="22"/>
+      <c r="G26" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C27" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="22"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="29"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33"/>
+    </row>
+    <row r="29" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="12">
         <v>4</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D30" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:9" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12">
+    <row r="31" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:9" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="12">
         <v>5</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D32" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="2:9" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="12" t="s">
+    <row r="33" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:8" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C34" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D34" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="H32" s="25"/>
-    </row>
-    <row r="33" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H33" s="25"/>
-    </row>
-    <row r="34" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="H34" s="25"/>
-    </row>
-    <row r="35" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H35" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="H36" s="25"/>
-    </row>
-    <row r="37" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H37" s="23"/>
+    </row>
+    <row r="38" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="18"/>
+      <c r="H38" s="23"/>
+    </row>
+    <row r="39" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H39" s="23"/>
+    </row>
+    <row r="40" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="H40" s="23"/>
+    </row>
+    <row r="41" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="23"/>
+    </row>
+    <row r="42" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="H42" s="23"/>
+    </row>
+    <row r="43" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H43" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="H44" s="23"/>
+    </row>
+    <row r="45" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>